<commit_message>
try to push again
</commit_message>
<xml_diff>
--- a/data/monitoringPhenology/2025BudburstToBudset.xlsx
+++ b/data/monitoringPhenology/2025BudburstToBudset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/monitoringPhenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD26351-7F50-A74F-86CC-0DB68861E8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA02D4C-221A-4E4D-984F-831C0BAE0FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="-2480" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="phenological_monitoring" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">phenological_monitoring!$A$1:$E$621</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">phenological_monitoring!$A$1:$E$620</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2492" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2488" uniqueCount="650">
   <si>
     <t>tree_ID</t>
   </si>
@@ -1623,9 +1623,6 @@
   </si>
   <si>
     <t>Quma_WarmS/WarmF_B1_R5</t>
-  </si>
-  <si>
-    <t>Quma_WarmS/WarmF_B2_R6</t>
   </si>
   <si>
     <t>Quma_WarmS/WarmF_B2_R7</t>
@@ -2637,8 +2634,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C09BEA22-6943-C148-893B-096C13910EF5}" name="Table1" displayName="Table1" ref="A1:I621" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I621" xr:uid="{C09BEA22-6943-C148-893B-096C13910EF5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C09BEA22-6943-C148-893B-096C13910EF5}" name="Table1" displayName="Table1" ref="A1:I620" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I620" xr:uid="{C09BEA22-6943-C148-893B-096C13910EF5}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{6B7D526F-2D16-104C-916C-5A8D81E298F2}" name="tree_ID" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{E0C9A5F2-2115-B942-922F-AAB1B58E7971}" name="bloc" dataDxfId="7"/>
@@ -2971,11 +2968,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I621"/>
+  <dimension ref="A1:I620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A471" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A494" zoomScale="226" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E486" sqref="E486"/>
+      <selection pane="topRight" activeCell="D508" sqref="D508"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3004,13 +3001,13 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>645</v>
+      </c>
+      <c r="H1" t="s">
         <v>646</v>
       </c>
-      <c r="H1" t="s">
-        <v>647</v>
-      </c>
       <c r="I1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -13352,7 +13349,7 @@
         <v>382</v>
       </c>
       <c r="F399" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G399">
         <v>0</v>
@@ -13459,7 +13456,7 @@
         <v>382</v>
       </c>
       <c r="F403" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I403"/>
     </row>
@@ -14260,7 +14257,7 @@
         <v>382</v>
       </c>
       <c r="F434" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G434">
         <v>0</v>
@@ -16253,7 +16250,7 @@
         <v>533</v>
       </c>
       <c r="B511">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C511" t="s">
         <v>73</v>
@@ -16383,10 +16380,10 @@
         <v>538</v>
       </c>
       <c r="B516">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C516" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D516" t="s">
         <v>464</v>
@@ -16513,7 +16510,7 @@
         <v>543</v>
       </c>
       <c r="B521">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C521" t="s">
         <v>89</v>
@@ -16643,7 +16640,7 @@
         <v>548</v>
       </c>
       <c r="B526">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C526" t="s">
         <v>89</v>
@@ -16773,16 +16770,16 @@
         <v>553</v>
       </c>
       <c r="B531">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C531" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D531" t="s">
-        <v>464</v>
+        <v>554</v>
       </c>
       <c r="E531" t="s">
-        <v>465</v>
+        <v>555</v>
       </c>
       <c r="G531">
         <v>0</v>
@@ -16796,7 +16793,7 @@
     </row>
     <row r="532" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B532">
         <v>1</v>
@@ -16805,10 +16802,10 @@
         <v>7</v>
       </c>
       <c r="D532" t="s">
+        <v>554</v>
+      </c>
+      <c r="E532" t="s">
         <v>555</v>
-      </c>
-      <c r="E532" t="s">
-        <v>556</v>
       </c>
       <c r="G532">
         <v>0</v>
@@ -16831,10 +16828,10 @@
         <v>7</v>
       </c>
       <c r="D533" t="s">
+        <v>554</v>
+      </c>
+      <c r="E533" t="s">
         <v>555</v>
-      </c>
-      <c r="E533" t="s">
-        <v>556</v>
       </c>
       <c r="G533">
         <v>0</v>
@@ -16857,10 +16854,10 @@
         <v>7</v>
       </c>
       <c r="D534" t="s">
+        <v>554</v>
+      </c>
+      <c r="E534" t="s">
         <v>555</v>
-      </c>
-      <c r="E534" t="s">
-        <v>556</v>
       </c>
       <c r="G534">
         <v>0</v>
@@ -16883,10 +16880,10 @@
         <v>7</v>
       </c>
       <c r="D535" t="s">
+        <v>554</v>
+      </c>
+      <c r="E535" t="s">
         <v>555</v>
-      </c>
-      <c r="E535" t="s">
-        <v>556</v>
       </c>
       <c r="G535">
         <v>0</v>
@@ -16903,16 +16900,16 @@
         <v>560</v>
       </c>
       <c r="B536">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C536" t="s">
         <v>7</v>
       </c>
       <c r="D536" t="s">
+        <v>554</v>
+      </c>
+      <c r="E536" t="s">
         <v>555</v>
-      </c>
-      <c r="E536" t="s">
-        <v>556</v>
       </c>
       <c r="G536">
         <v>0</v>
@@ -16935,10 +16932,10 @@
         <v>7</v>
       </c>
       <c r="D537" t="s">
+        <v>554</v>
+      </c>
+      <c r="E537" t="s">
         <v>555</v>
-      </c>
-      <c r="E537" t="s">
-        <v>556</v>
       </c>
       <c r="G537">
         <v>0</v>
@@ -16961,10 +16958,10 @@
         <v>7</v>
       </c>
       <c r="D538" t="s">
+        <v>554</v>
+      </c>
+      <c r="E538" t="s">
         <v>555</v>
-      </c>
-      <c r="E538" t="s">
-        <v>556</v>
       </c>
       <c r="G538">
         <v>0</v>
@@ -16987,10 +16984,10 @@
         <v>7</v>
       </c>
       <c r="D539" t="s">
+        <v>554</v>
+      </c>
+      <c r="E539" t="s">
         <v>555</v>
-      </c>
-      <c r="E539" t="s">
-        <v>556</v>
       </c>
       <c r="G539">
         <v>0</v>
@@ -17013,10 +17010,10 @@
         <v>7</v>
       </c>
       <c r="D540" t="s">
+        <v>554</v>
+      </c>
+      <c r="E540" t="s">
         <v>555</v>
-      </c>
-      <c r="E540" t="s">
-        <v>556</v>
       </c>
       <c r="G540">
         <v>0</v>
@@ -17033,16 +17030,16 @@
         <v>565</v>
       </c>
       <c r="B541">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C541" t="s">
         <v>7</v>
       </c>
       <c r="D541" t="s">
+        <v>554</v>
+      </c>
+      <c r="E541" t="s">
         <v>555</v>
-      </c>
-      <c r="E541" t="s">
-        <v>556</v>
       </c>
       <c r="G541">
         <v>0</v>
@@ -17065,10 +17062,10 @@
         <v>7</v>
       </c>
       <c r="D542" t="s">
+        <v>554</v>
+      </c>
+      <c r="E542" t="s">
         <v>555</v>
-      </c>
-      <c r="E542" t="s">
-        <v>556</v>
       </c>
       <c r="G542">
         <v>0</v>
@@ -17091,10 +17088,10 @@
         <v>7</v>
       </c>
       <c r="D543" t="s">
+        <v>554</v>
+      </c>
+      <c r="E543" t="s">
         <v>555</v>
-      </c>
-      <c r="E543" t="s">
-        <v>556</v>
       </c>
       <c r="G543">
         <v>0</v>
@@ -17117,10 +17114,10 @@
         <v>7</v>
       </c>
       <c r="D544" t="s">
+        <v>554</v>
+      </c>
+      <c r="E544" t="s">
         <v>555</v>
-      </c>
-      <c r="E544" t="s">
-        <v>556</v>
       </c>
       <c r="G544">
         <v>0</v>
@@ -17143,10 +17140,10 @@
         <v>7</v>
       </c>
       <c r="D545" t="s">
+        <v>554</v>
+      </c>
+      <c r="E545" t="s">
         <v>555</v>
-      </c>
-      <c r="E545" t="s">
-        <v>556</v>
       </c>
       <c r="G545">
         <v>0</v>
@@ -17163,16 +17160,16 @@
         <v>570</v>
       </c>
       <c r="B546">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C546" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D546" t="s">
+        <v>554</v>
+      </c>
+      <c r="E546" t="s">
         <v>555</v>
-      </c>
-      <c r="E546" t="s">
-        <v>556</v>
       </c>
       <c r="G546">
         <v>0</v>
@@ -17195,10 +17192,10 @@
         <v>25</v>
       </c>
       <c r="D547" t="s">
+        <v>554</v>
+      </c>
+      <c r="E547" t="s">
         <v>555</v>
-      </c>
-      <c r="E547" t="s">
-        <v>556</v>
       </c>
       <c r="G547">
         <v>0</v>
@@ -17221,10 +17218,10 @@
         <v>25</v>
       </c>
       <c r="D548" t="s">
+        <v>554</v>
+      </c>
+      <c r="E548" t="s">
         <v>555</v>
-      </c>
-      <c r="E548" t="s">
-        <v>556</v>
       </c>
       <c r="G548">
         <v>0</v>
@@ -17247,10 +17244,10 @@
         <v>25</v>
       </c>
       <c r="D549" t="s">
+        <v>554</v>
+      </c>
+      <c r="E549" t="s">
         <v>555</v>
-      </c>
-      <c r="E549" t="s">
-        <v>556</v>
       </c>
       <c r="G549">
         <v>0</v>
@@ -17273,10 +17270,10 @@
         <v>25</v>
       </c>
       <c r="D550" t="s">
+        <v>554</v>
+      </c>
+      <c r="E550" t="s">
         <v>555</v>
-      </c>
-      <c r="E550" t="s">
-        <v>556</v>
       </c>
       <c r="G550">
         <v>0</v>
@@ -17293,16 +17290,16 @@
         <v>575</v>
       </c>
       <c r="B551">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C551" t="s">
         <v>25</v>
       </c>
       <c r="D551" t="s">
+        <v>554</v>
+      </c>
+      <c r="E551" t="s">
         <v>555</v>
-      </c>
-      <c r="E551" t="s">
-        <v>556</v>
       </c>
       <c r="G551">
         <v>0</v>
@@ -17325,10 +17322,10 @@
         <v>25</v>
       </c>
       <c r="D552" t="s">
+        <v>554</v>
+      </c>
+      <c r="E552" t="s">
         <v>555</v>
-      </c>
-      <c r="E552" t="s">
-        <v>556</v>
       </c>
       <c r="G552">
         <v>0</v>
@@ -17351,10 +17348,10 @@
         <v>25</v>
       </c>
       <c r="D553" t="s">
+        <v>554</v>
+      </c>
+      <c r="E553" t="s">
         <v>555</v>
-      </c>
-      <c r="E553" t="s">
-        <v>556</v>
       </c>
       <c r="G553">
         <v>0</v>
@@ -17377,10 +17374,10 @@
         <v>25</v>
       </c>
       <c r="D554" t="s">
+        <v>554</v>
+      </c>
+      <c r="E554" t="s">
         <v>555</v>
-      </c>
-      <c r="E554" t="s">
-        <v>556</v>
       </c>
       <c r="G554">
         <v>0</v>
@@ -17403,10 +17400,10 @@
         <v>25</v>
       </c>
       <c r="D555" t="s">
+        <v>554</v>
+      </c>
+      <c r="E555" t="s">
         <v>555</v>
-      </c>
-      <c r="E555" t="s">
-        <v>556</v>
       </c>
       <c r="G555">
         <v>0</v>
@@ -17423,16 +17420,16 @@
         <v>580</v>
       </c>
       <c r="B556">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C556" t="s">
         <v>25</v>
       </c>
       <c r="D556" t="s">
+        <v>554</v>
+      </c>
+      <c r="E556" t="s">
         <v>555</v>
-      </c>
-      <c r="E556" t="s">
-        <v>556</v>
       </c>
       <c r="G556">
         <v>0</v>
@@ -17455,10 +17452,10 @@
         <v>25</v>
       </c>
       <c r="D557" t="s">
+        <v>554</v>
+      </c>
+      <c r="E557" t="s">
         <v>555</v>
-      </c>
-      <c r="E557" t="s">
-        <v>556</v>
       </c>
       <c r="G557">
         <v>0</v>
@@ -17481,10 +17478,10 @@
         <v>25</v>
       </c>
       <c r="D558" t="s">
+        <v>554</v>
+      </c>
+      <c r="E558" t="s">
         <v>555</v>
-      </c>
-      <c r="E558" t="s">
-        <v>556</v>
       </c>
       <c r="G558">
         <v>0</v>
@@ -17507,10 +17504,10 @@
         <v>25</v>
       </c>
       <c r="D559" t="s">
+        <v>554</v>
+      </c>
+      <c r="E559" t="s">
         <v>555</v>
-      </c>
-      <c r="E559" t="s">
-        <v>556</v>
       </c>
       <c r="G559">
         <v>0</v>
@@ -17533,10 +17530,10 @@
         <v>25</v>
       </c>
       <c r="D560" t="s">
+        <v>554</v>
+      </c>
+      <c r="E560" t="s">
         <v>555</v>
-      </c>
-      <c r="E560" t="s">
-        <v>556</v>
       </c>
       <c r="G560">
         <v>0</v>
@@ -17553,16 +17550,16 @@
         <v>585</v>
       </c>
       <c r="B561">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C561" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D561" t="s">
+        <v>554</v>
+      </c>
+      <c r="E561" t="s">
         <v>555</v>
-      </c>
-      <c r="E561" t="s">
-        <v>556</v>
       </c>
       <c r="G561">
         <v>0</v>
@@ -17585,10 +17582,10 @@
         <v>41</v>
       </c>
       <c r="D562" t="s">
+        <v>554</v>
+      </c>
+      <c r="E562" t="s">
         <v>555</v>
-      </c>
-      <c r="E562" t="s">
-        <v>556</v>
       </c>
       <c r="G562">
         <v>0</v>
@@ -17611,10 +17608,10 @@
         <v>41</v>
       </c>
       <c r="D563" t="s">
+        <v>554</v>
+      </c>
+      <c r="E563" t="s">
         <v>555</v>
-      </c>
-      <c r="E563" t="s">
-        <v>556</v>
       </c>
       <c r="G563">
         <v>0</v>
@@ -17637,10 +17634,10 @@
         <v>41</v>
       </c>
       <c r="D564" t="s">
+        <v>554</v>
+      </c>
+      <c r="E564" t="s">
         <v>555</v>
-      </c>
-      <c r="E564" t="s">
-        <v>556</v>
       </c>
       <c r="G564">
         <v>0</v>
@@ -17663,10 +17660,10 @@
         <v>41</v>
       </c>
       <c r="D565" t="s">
+        <v>554</v>
+      </c>
+      <c r="E565" t="s">
         <v>555</v>
-      </c>
-      <c r="E565" t="s">
-        <v>556</v>
       </c>
       <c r="G565">
         <v>0</v>
@@ -17683,16 +17680,16 @@
         <v>590</v>
       </c>
       <c r="B566">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C566" t="s">
         <v>41</v>
       </c>
       <c r="D566" t="s">
+        <v>554</v>
+      </c>
+      <c r="E566" t="s">
         <v>555</v>
-      </c>
-      <c r="E566" t="s">
-        <v>556</v>
       </c>
       <c r="G566">
         <v>0</v>
@@ -17715,10 +17712,10 @@
         <v>41</v>
       </c>
       <c r="D567" t="s">
+        <v>554</v>
+      </c>
+      <c r="E567" t="s">
         <v>555</v>
-      </c>
-      <c r="E567" t="s">
-        <v>556</v>
       </c>
       <c r="G567">
         <v>0</v>
@@ -17741,10 +17738,10 @@
         <v>41</v>
       </c>
       <c r="D568" t="s">
+        <v>554</v>
+      </c>
+      <c r="E568" t="s">
         <v>555</v>
-      </c>
-      <c r="E568" t="s">
-        <v>556</v>
       </c>
       <c r="G568">
         <v>0</v>
@@ -17767,10 +17764,10 @@
         <v>41</v>
       </c>
       <c r="D569" t="s">
+        <v>554</v>
+      </c>
+      <c r="E569" t="s">
         <v>555</v>
-      </c>
-      <c r="E569" t="s">
-        <v>556</v>
       </c>
       <c r="G569">
         <v>0</v>
@@ -17793,10 +17790,10 @@
         <v>41</v>
       </c>
       <c r="D570" t="s">
+        <v>554</v>
+      </c>
+      <c r="E570" t="s">
         <v>555</v>
-      </c>
-      <c r="E570" t="s">
-        <v>556</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -17813,16 +17810,16 @@
         <v>595</v>
       </c>
       <c r="B571">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C571" t="s">
         <v>41</v>
       </c>
       <c r="D571" t="s">
+        <v>554</v>
+      </c>
+      <c r="E571" t="s">
         <v>555</v>
-      </c>
-      <c r="E571" t="s">
-        <v>556</v>
       </c>
       <c r="G571">
         <v>0</v>
@@ -17845,10 +17842,10 @@
         <v>41</v>
       </c>
       <c r="D572" t="s">
+        <v>554</v>
+      </c>
+      <c r="E572" t="s">
         <v>555</v>
-      </c>
-      <c r="E572" t="s">
-        <v>556</v>
       </c>
       <c r="G572">
         <v>0</v>
@@ -17871,10 +17868,10 @@
         <v>41</v>
       </c>
       <c r="D573" t="s">
+        <v>554</v>
+      </c>
+      <c r="E573" t="s">
         <v>555</v>
-      </c>
-      <c r="E573" t="s">
-        <v>556</v>
       </c>
       <c r="G573">
         <v>0</v>
@@ -17897,10 +17894,10 @@
         <v>41</v>
       </c>
       <c r="D574" t="s">
+        <v>554</v>
+      </c>
+      <c r="E574" t="s">
         <v>555</v>
-      </c>
-      <c r="E574" t="s">
-        <v>556</v>
       </c>
       <c r="G574">
         <v>0</v>
@@ -17923,10 +17920,10 @@
         <v>41</v>
       </c>
       <c r="D575" t="s">
+        <v>554</v>
+      </c>
+      <c r="E575" t="s">
         <v>555</v>
-      </c>
-      <c r="E575" t="s">
-        <v>556</v>
       </c>
       <c r="G575">
         <v>0</v>
@@ -17943,16 +17940,16 @@
         <v>600</v>
       </c>
       <c r="B576">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C576" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="D576" t="s">
+        <v>554</v>
+      </c>
+      <c r="E576" t="s">
         <v>555</v>
-      </c>
-      <c r="E576" t="s">
-        <v>556</v>
       </c>
       <c r="G576">
         <v>0</v>
@@ -17975,10 +17972,10 @@
         <v>57</v>
       </c>
       <c r="D577" t="s">
+        <v>554</v>
+      </c>
+      <c r="E577" t="s">
         <v>555</v>
-      </c>
-      <c r="E577" t="s">
-        <v>556</v>
       </c>
       <c r="G577">
         <v>0</v>
@@ -18001,10 +17998,10 @@
         <v>57</v>
       </c>
       <c r="D578" t="s">
+        <v>554</v>
+      </c>
+      <c r="E578" t="s">
         <v>555</v>
-      </c>
-      <c r="E578" t="s">
-        <v>556</v>
       </c>
       <c r="G578">
         <v>0</v>
@@ -18027,10 +18024,10 @@
         <v>57</v>
       </c>
       <c r="D579" t="s">
+        <v>554</v>
+      </c>
+      <c r="E579" t="s">
         <v>555</v>
-      </c>
-      <c r="E579" t="s">
-        <v>556</v>
       </c>
       <c r="G579">
         <v>0</v>
@@ -18053,10 +18050,10 @@
         <v>57</v>
       </c>
       <c r="D580" t="s">
+        <v>554</v>
+      </c>
+      <c r="E580" t="s">
         <v>555</v>
-      </c>
-      <c r="E580" t="s">
-        <v>556</v>
       </c>
       <c r="G580">
         <v>0</v>
@@ -18073,16 +18070,16 @@
         <v>605</v>
       </c>
       <c r="B581">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C581" t="s">
         <v>57</v>
       </c>
       <c r="D581" t="s">
+        <v>554</v>
+      </c>
+      <c r="E581" t="s">
         <v>555</v>
-      </c>
-      <c r="E581" t="s">
-        <v>556</v>
       </c>
       <c r="G581">
         <v>0</v>
@@ -18105,10 +18102,10 @@
         <v>57</v>
       </c>
       <c r="D582" t="s">
+        <v>554</v>
+      </c>
+      <c r="E582" t="s">
         <v>555</v>
-      </c>
-      <c r="E582" t="s">
-        <v>556</v>
       </c>
       <c r="G582">
         <v>0</v>
@@ -18131,10 +18128,10 @@
         <v>57</v>
       </c>
       <c r="D583" t="s">
+        <v>554</v>
+      </c>
+      <c r="E583" t="s">
         <v>555</v>
-      </c>
-      <c r="E583" t="s">
-        <v>556</v>
       </c>
       <c r="G583">
         <v>0</v>
@@ -18157,10 +18154,10 @@
         <v>57</v>
       </c>
       <c r="D584" t="s">
+        <v>554</v>
+      </c>
+      <c r="E584" t="s">
         <v>555</v>
-      </c>
-      <c r="E584" t="s">
-        <v>556</v>
       </c>
       <c r="G584">
         <v>0</v>
@@ -18183,10 +18180,10 @@
         <v>57</v>
       </c>
       <c r="D585" t="s">
+        <v>554</v>
+      </c>
+      <c r="E585" t="s">
         <v>555</v>
-      </c>
-      <c r="E585" t="s">
-        <v>556</v>
       </c>
       <c r="G585">
         <v>0</v>
@@ -18203,16 +18200,16 @@
         <v>610</v>
       </c>
       <c r="B586">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C586" t="s">
         <v>57</v>
       </c>
       <c r="D586" t="s">
+        <v>554</v>
+      </c>
+      <c r="E586" t="s">
         <v>555</v>
-      </c>
-      <c r="E586" t="s">
-        <v>556</v>
       </c>
       <c r="G586">
         <v>0</v>
@@ -18235,10 +18232,10 @@
         <v>57</v>
       </c>
       <c r="D587" t="s">
+        <v>554</v>
+      </c>
+      <c r="E587" t="s">
         <v>555</v>
-      </c>
-      <c r="E587" t="s">
-        <v>556</v>
       </c>
       <c r="G587">
         <v>0</v>
@@ -18261,10 +18258,10 @@
         <v>57</v>
       </c>
       <c r="D588" t="s">
+        <v>554</v>
+      </c>
+      <c r="E588" t="s">
         <v>555</v>
-      </c>
-      <c r="E588" t="s">
-        <v>556</v>
       </c>
       <c r="G588">
         <v>0</v>
@@ -18287,10 +18284,10 @@
         <v>57</v>
       </c>
       <c r="D589" t="s">
+        <v>554</v>
+      </c>
+      <c r="E589" t="s">
         <v>555</v>
-      </c>
-      <c r="E589" t="s">
-        <v>556</v>
       </c>
       <c r="G589">
         <v>0</v>
@@ -18313,10 +18310,10 @@
         <v>57</v>
       </c>
       <c r="D590" t="s">
+        <v>554</v>
+      </c>
+      <c r="E590" t="s">
         <v>555</v>
-      </c>
-      <c r="E590" t="s">
-        <v>556</v>
       </c>
       <c r="G590">
         <v>0</v>
@@ -18333,16 +18330,16 @@
         <v>615</v>
       </c>
       <c r="B591">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C591" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D591" t="s">
+        <v>554</v>
+      </c>
+      <c r="E591" t="s">
         <v>555</v>
-      </c>
-      <c r="E591" t="s">
-        <v>556</v>
       </c>
       <c r="G591">
         <v>0</v>
@@ -18365,10 +18362,10 @@
         <v>73</v>
       </c>
       <c r="D592" t="s">
+        <v>554</v>
+      </c>
+      <c r="E592" t="s">
         <v>555</v>
-      </c>
-      <c r="E592" t="s">
-        <v>556</v>
       </c>
       <c r="G592">
         <v>0</v>
@@ -18391,10 +18388,10 @@
         <v>73</v>
       </c>
       <c r="D593" t="s">
+        <v>554</v>
+      </c>
+      <c r="E593" t="s">
         <v>555</v>
-      </c>
-      <c r="E593" t="s">
-        <v>556</v>
       </c>
       <c r="G593">
         <v>0</v>
@@ -18417,10 +18414,10 @@
         <v>73</v>
       </c>
       <c r="D594" t="s">
+        <v>554</v>
+      </c>
+      <c r="E594" t="s">
         <v>555</v>
-      </c>
-      <c r="E594" t="s">
-        <v>556</v>
       </c>
       <c r="G594">
         <v>0</v>
@@ -18443,10 +18440,10 @@
         <v>73</v>
       </c>
       <c r="D595" t="s">
+        <v>554</v>
+      </c>
+      <c r="E595" t="s">
         <v>555</v>
-      </c>
-      <c r="E595" t="s">
-        <v>556</v>
       </c>
       <c r="G595">
         <v>0</v>
@@ -18463,16 +18460,16 @@
         <v>620</v>
       </c>
       <c r="B596">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C596" t="s">
         <v>73</v>
       </c>
       <c r="D596" t="s">
+        <v>554</v>
+      </c>
+      <c r="E596" t="s">
         <v>555</v>
-      </c>
-      <c r="E596" t="s">
-        <v>556</v>
       </c>
       <c r="G596">
         <v>0</v>
@@ -18495,10 +18492,10 @@
         <v>73</v>
       </c>
       <c r="D597" t="s">
+        <v>554</v>
+      </c>
+      <c r="E597" t="s">
         <v>555</v>
-      </c>
-      <c r="E597" t="s">
-        <v>556</v>
       </c>
       <c r="G597">
         <v>0</v>
@@ -18521,10 +18518,10 @@
         <v>73</v>
       </c>
       <c r="D598" t="s">
+        <v>554</v>
+      </c>
+      <c r="E598" t="s">
         <v>555</v>
-      </c>
-      <c r="E598" t="s">
-        <v>556</v>
       </c>
       <c r="G598">
         <v>0</v>
@@ -18547,10 +18544,10 @@
         <v>73</v>
       </c>
       <c r="D599" t="s">
+        <v>554</v>
+      </c>
+      <c r="E599" t="s">
         <v>555</v>
-      </c>
-      <c r="E599" t="s">
-        <v>556</v>
       </c>
       <c r="G599">
         <v>0</v>
@@ -18573,10 +18570,10 @@
         <v>73</v>
       </c>
       <c r="D600" t="s">
+        <v>554</v>
+      </c>
+      <c r="E600" t="s">
         <v>555</v>
-      </c>
-      <c r="E600" t="s">
-        <v>556</v>
       </c>
       <c r="G600">
         <v>0</v>
@@ -18593,16 +18590,16 @@
         <v>625</v>
       </c>
       <c r="B601">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C601" t="s">
         <v>73</v>
       </c>
       <c r="D601" t="s">
+        <v>554</v>
+      </c>
+      <c r="E601" t="s">
         <v>555</v>
-      </c>
-      <c r="E601" t="s">
-        <v>556</v>
       </c>
       <c r="G601">
         <v>0</v>
@@ -18625,10 +18622,10 @@
         <v>73</v>
       </c>
       <c r="D602" t="s">
+        <v>554</v>
+      </c>
+      <c r="E602" t="s">
         <v>555</v>
-      </c>
-      <c r="E602" t="s">
-        <v>556</v>
       </c>
       <c r="G602">
         <v>0</v>
@@ -18651,10 +18648,10 @@
         <v>73</v>
       </c>
       <c r="D603" t="s">
+        <v>554</v>
+      </c>
+      <c r="E603" t="s">
         <v>555</v>
-      </c>
-      <c r="E603" t="s">
-        <v>556</v>
       </c>
       <c r="G603">
         <v>0</v>
@@ -18677,10 +18674,10 @@
         <v>73</v>
       </c>
       <c r="D604" t="s">
+        <v>554</v>
+      </c>
+      <c r="E604" t="s">
         <v>555</v>
-      </c>
-      <c r="E604" t="s">
-        <v>556</v>
       </c>
       <c r="G604">
         <v>0</v>
@@ -18703,10 +18700,10 @@
         <v>73</v>
       </c>
       <c r="D605" t="s">
+        <v>554</v>
+      </c>
+      <c r="E605" t="s">
         <v>555</v>
-      </c>
-      <c r="E605" t="s">
-        <v>556</v>
       </c>
       <c r="G605">
         <v>0</v>
@@ -18723,16 +18720,16 @@
         <v>630</v>
       </c>
       <c r="B606">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C606" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D606" t="s">
+        <v>554</v>
+      </c>
+      <c r="E606" t="s">
         <v>555</v>
-      </c>
-      <c r="E606" t="s">
-        <v>556</v>
       </c>
       <c r="G606">
         <v>0</v>
@@ -18755,10 +18752,10 @@
         <v>89</v>
       </c>
       <c r="D607" t="s">
+        <v>554</v>
+      </c>
+      <c r="E607" t="s">
         <v>555</v>
-      </c>
-      <c r="E607" t="s">
-        <v>556</v>
       </c>
       <c r="G607">
         <v>0</v>
@@ -18781,10 +18778,10 @@
         <v>89</v>
       </c>
       <c r="D608" t="s">
+        <v>554</v>
+      </c>
+      <c r="E608" t="s">
         <v>555</v>
-      </c>
-      <c r="E608" t="s">
-        <v>556</v>
       </c>
       <c r="G608">
         <v>0</v>
@@ -18807,10 +18804,10 @@
         <v>89</v>
       </c>
       <c r="D609" t="s">
+        <v>554</v>
+      </c>
+      <c r="E609" t="s">
         <v>555</v>
-      </c>
-      <c r="E609" t="s">
-        <v>556</v>
       </c>
       <c r="G609">
         <v>0</v>
@@ -18833,10 +18830,10 @@
         <v>89</v>
       </c>
       <c r="D610" t="s">
+        <v>554</v>
+      </c>
+      <c r="E610" t="s">
         <v>555</v>
-      </c>
-      <c r="E610" t="s">
-        <v>556</v>
       </c>
       <c r="G610">
         <v>0</v>
@@ -18853,16 +18850,16 @@
         <v>635</v>
       </c>
       <c r="B611">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C611" t="s">
         <v>89</v>
       </c>
       <c r="D611" t="s">
+        <v>554</v>
+      </c>
+      <c r="E611" t="s">
         <v>555</v>
-      </c>
-      <c r="E611" t="s">
-        <v>556</v>
       </c>
       <c r="G611">
         <v>0</v>
@@ -18885,10 +18882,10 @@
         <v>89</v>
       </c>
       <c r="D612" t="s">
+        <v>554</v>
+      </c>
+      <c r="E612" t="s">
         <v>555</v>
-      </c>
-      <c r="E612" t="s">
-        <v>556</v>
       </c>
       <c r="G612">
         <v>0</v>
@@ -18911,10 +18908,10 @@
         <v>89</v>
       </c>
       <c r="D613" t="s">
+        <v>554</v>
+      </c>
+      <c r="E613" t="s">
         <v>555</v>
-      </c>
-      <c r="E613" t="s">
-        <v>556</v>
       </c>
       <c r="G613">
         <v>0</v>
@@ -18937,10 +18934,10 @@
         <v>89</v>
       </c>
       <c r="D614" t="s">
+        <v>554</v>
+      </c>
+      <c r="E614" t="s">
         <v>555</v>
-      </c>
-      <c r="E614" t="s">
-        <v>556</v>
       </c>
       <c r="G614">
         <v>0</v>
@@ -18963,10 +18960,10 @@
         <v>89</v>
       </c>
       <c r="D615" t="s">
+        <v>554</v>
+      </c>
+      <c r="E615" t="s">
         <v>555</v>
-      </c>
-      <c r="E615" t="s">
-        <v>556</v>
       </c>
       <c r="G615">
         <v>0</v>
@@ -18983,16 +18980,16 @@
         <v>640</v>
       </c>
       <c r="B616">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C616" t="s">
         <v>89</v>
       </c>
       <c r="D616" t="s">
+        <v>554</v>
+      </c>
+      <c r="E616" t="s">
         <v>555</v>
-      </c>
-      <c r="E616" t="s">
-        <v>556</v>
       </c>
       <c r="G616">
         <v>0</v>
@@ -19015,10 +19012,10 @@
         <v>89</v>
       </c>
       <c r="D617" t="s">
+        <v>554</v>
+      </c>
+      <c r="E617" t="s">
         <v>555</v>
-      </c>
-      <c r="E617" t="s">
-        <v>556</v>
       </c>
       <c r="G617">
         <v>0</v>
@@ -19041,10 +19038,10 @@
         <v>89</v>
       </c>
       <c r="D618" t="s">
+        <v>554</v>
+      </c>
+      <c r="E618" t="s">
         <v>555</v>
-      </c>
-      <c r="E618" t="s">
-        <v>556</v>
       </c>
       <c r="G618">
         <v>0</v>
@@ -19067,10 +19064,10 @@
         <v>89</v>
       </c>
       <c r="D619" t="s">
+        <v>554</v>
+      </c>
+      <c r="E619" t="s">
         <v>555</v>
-      </c>
-      <c r="E619" t="s">
-        <v>556</v>
       </c>
       <c r="G619">
         <v>0</v>
@@ -19093,11 +19090,11 @@
         <v>89</v>
       </c>
       <c r="D620" t="s">
+        <v>554</v>
+      </c>
+      <c r="E620" t="s">
         <v>555</v>
       </c>
-      <c r="E620" t="s">
-        <v>556</v>
-      </c>
       <c r="G620">
         <v>0</v>
       </c>
@@ -19105,32 +19102,6 @@
         <v>0</v>
       </c>
       <c r="I620">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="621" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A621" t="s">
-        <v>645</v>
-      </c>
-      <c r="B621">
-        <v>3</v>
-      </c>
-      <c r="C621" t="s">
-        <v>89</v>
-      </c>
-      <c r="D621" t="s">
-        <v>555</v>
-      </c>
-      <c r="E621" t="s">
-        <v>556</v>
-      </c>
-      <c r="G621">
-        <v>0</v>
-      </c>
-      <c r="H621">
-        <v>0</v>
-      </c>
-      <c r="I621">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed acne that I messed up
</commit_message>
<xml_diff>
--- a/data/monitoringPhenology/2025BudburstToBudset.xlsx
+++ b/data/monitoringPhenology/2025BudburstToBudset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/monitoringPhenology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1267BB53-AF7E-0D44-A79C-78C1471C3201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FE2F22-5EFD-3246-933B-85958342FCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="740" windowWidth="19980" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phenological_monitoring" sheetId="1" r:id="rId1"/>
@@ -2513,10 +2513,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -3037,9 +3038,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" zoomScale="200" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K274" sqref="K274"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="200" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4827,11 +4828,11 @@
       <c r="J47">
         <v>0</v>
       </c>
-      <c r="K47">
-        <v>1</v>
-      </c>
-      <c r="L47">
-        <v>1</v>
+      <c r="K47" s="3">
+        <v>0</v>
+      </c>
+      <c r="L47" s="3">
+        <v>0</v>
       </c>
       <c r="M47">
         <v>1</v>
@@ -4904,10 +4905,10 @@
         <v>0</v>
       </c>
       <c r="K49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49">
         <v>1</v>

</xml_diff>